<commit_message>
add escala in pionero format
</commit_message>
<xml_diff>
--- a/data/PIONERO FEB26.xlsx
+++ b/data/PIONERO FEB26.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Programing Clients\BuscadorProdProveedores\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A988FEB6-B313-4BAE-8105-800C8CFFAFB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{921FC086-54E5-43EC-8A54-1DC74886337A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D2740E0C-77BB-4718-B64A-FAB77F9257AD}"/>
   </bookViews>
@@ -5822,31 +5822,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="20">
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FFFFFFFF"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFFFFFFF"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b/>
@@ -6015,6 +5990,31 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FFFFFFFF"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFFFFFFF"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -6029,18 +6029,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5079A2E7-88B6-49BB-A159-532ACD082401}" name="Lista" displayName="Lista" ref="A1:J1801" totalsRowCount="1" headerRowDxfId="0" headerRowBorderDxfId="19" tableBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5079A2E7-88B6-49BB-A159-532ACD082401}" name="Lista" displayName="Lista" ref="A1:J1801" totalsRowCount="1" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17">
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{0EF8E220-C220-4427-8D72-E6DE331EAF62}" name="CODIGO" dataDxfId="17" totalsRowDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{0EF8E220-C220-4427-8D72-E6DE331EAF62}" name="CODIGO" dataDxfId="16" totalsRowDxfId="7"/>
     <tableColumn id="2" xr3:uid="{2C3202EC-8243-4339-AE8F-109F865E98C1}" name="NOMBRE"/>
     <tableColumn id="4" xr3:uid="{0D94A12C-880F-49E4-959D-DCCBFC888DA1}" name="LABORATORIO"/>
-    <tableColumn id="5" xr3:uid="{EDACBF7E-2C4A-4114-8950-080F800D37EE}" name="PRECIO" dataDxfId="16" totalsRowDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{97ABCE63-25EE-4B16-83C0-DDC22BE54212}" name="Fecha Vcto" dataDxfId="15" totalsRowDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{D3ACC30E-F50F-4122-AB80-18EB8653FD76}" name="Escala" dataDxfId="14" totalsRowDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{7FF9917B-8BCB-4A9B-B357-85BBCCF19B51}" name="Precio Escala" dataDxfId="13" totalsRowDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{22EEB9CD-4B5C-4A8A-9F7B-E1DE416C44B4}" name="Meses vencimiento" dataDxfId="12" totalsRowDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{5F9B3D2E-0B54-4336-A714-69685363F2C9}" name="Cantida Pedido" dataDxfId="11" totalsRowDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{51E613C2-0C7C-4D94-AF2D-68D8F19F30A0}" name="Importe Total" totalsRowFunction="custom" dataDxfId="10" totalsRowDxfId="1">
+    <tableColumn id="5" xr3:uid="{EDACBF7E-2C4A-4114-8950-080F800D37EE}" name="PRECIO" dataDxfId="15" totalsRowDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{97ABCE63-25EE-4B16-83C0-DDC22BE54212}" name="Fecha Vcto" dataDxfId="14" totalsRowDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{D3ACC30E-F50F-4122-AB80-18EB8653FD76}" name="Escala" dataDxfId="13" totalsRowDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{7FF9917B-8BCB-4A9B-B357-85BBCCF19B51}" name="Precio Escala" dataDxfId="12" totalsRowDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{22EEB9CD-4B5C-4A8A-9F7B-E1DE416C44B4}" name="Meses vencimiento" dataDxfId="11" totalsRowDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{5F9B3D2E-0B54-4336-A714-69685363F2C9}" name="Cantida Pedido" dataDxfId="10" totalsRowDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{51E613C2-0C7C-4D94-AF2D-68D8F19F30A0}" name="Importe Total" totalsRowFunction="custom" dataDxfId="9" totalsRowDxfId="0">
       <calculatedColumnFormula>IF(Lista[[#This Row],[Escala]]="",Lista[[#This Row],[Cantida Pedido]]*Lista[[#This Row],[PRECIO]],IF(Lista[[#This Row],[Cantida Pedido]]&gt;=Lista[[#This Row],[Escala]],Lista[[#This Row],[Cantida Pedido]]*Lista[[#This Row],[Precio Escala]],Lista[[#This Row],[Cantida Pedido]]*Lista[[#This Row],[PRECIO]]))</calculatedColumnFormula>
       <totalsRowFormula>SUM(Lista[Importe Total])</totalsRowFormula>
     </tableColumn>
@@ -6349,7 +6349,7 @@
   <dimension ref="A1:J1801"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="B96" sqref="B96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -55324,7 +55324,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:J1800">
-    <cfRule type="expression" dxfId="9" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="2" stopIfTrue="1">
       <formula>$H2&lt;9</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>